<commit_message>
Completed adding all required lower division courses for cs majors
</commit_message>
<xml_diff>
--- a/CourseInformation.xlsx
+++ b/CourseInformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Latisha/Desktop/transferify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20C64E-9B23-FF43-B4E7-0C3EC74D566E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37856D1C-E57B-E949-A30A-FAE4EE04E56F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{799547F4-8573-6E46-8325-07C6A5C91E50}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Class Name</t>
   </si>
@@ -148,6 +148,48 @@
   </si>
   <si>
     <t>Discrete structures commonly used in computer science and mathematics, including sets and relations, permutations and combinations, graphs and trees, induction.</t>
+  </si>
+  <si>
+    <t>Physics 1A</t>
+  </si>
+  <si>
+    <t>Physics 1B</t>
+  </si>
+  <si>
+    <t>Physics 1C</t>
+  </si>
+  <si>
+    <t>Physics 4AL</t>
+  </si>
+  <si>
+    <t>Physics 4BL</t>
+  </si>
+  <si>
+    <t>Motion, Newton laws, work, energy, linear and angular momentum, rotation, equilibrium, gravitation.</t>
+  </si>
+  <si>
+    <t>Fluid mechanics, oscillation, mechanical waves, and sound. Electric charge, field and potential, capacitors, and dielectrics. Currents and resistance, direct-current circuits.</t>
+  </si>
+  <si>
+    <t>Magnetic fields, Ampere's law, Faraday's law, inductance, and alternating current circuits. Maxwell's equations, electromagnetic waves, light, geometrical optics, interference and diffraction.</t>
+  </si>
+  <si>
+    <t>Math 31A, Math 31B, Math 32A, Math 32B, Physics 1A</t>
+  </si>
+  <si>
+    <t>Math 31A, Math 31B, Math 32A, Math 32B, Math 33A, Physics 1A, Physics 1B</t>
+  </si>
+  <si>
+    <t>*Fulfills Same Requirement as Physics 4BL* Computerized measurements of uniform and accelerated motion, including oscillations. Analysis of data and comparison of results to predictions, including least-squares fitting. Conception, execution, and presentation of creative projects involving motion.</t>
+  </si>
+  <si>
+    <t>*Fulfills Same Requirement as Physics 4AL* Sound waves and electric circuits, taken by digital oscilloscopes and analyzed by Fourier transformation. Geometrical and physical optics. Conception, execution, and presentation of creative projects involving sound waves or electric circuits.</t>
+  </si>
+  <si>
+    <t>Math 31A, Math 31B, Math 32A, Physics 1A, Physics 1B</t>
+  </si>
+  <si>
+    <t>Math 31A, Math 31B, Math 32A, Math 32B, Math 33A, Physics 1A, Physics 1B, Physics 1C</t>
   </si>
 </sst>
 </file>
@@ -502,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB62880F-4327-8B45-B967-BF103E8C0F94}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,7 +558,7 @@
     <col min="3" max="3" width="6.1640625" customWidth="1"/>
     <col min="4" max="4" width="46.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="29.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -535,7 +577,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -555,7 +597,7 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -575,7 +617,7 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -595,7 +637,7 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -615,7 +657,7 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -635,7 +677,7 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -655,7 +697,7 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -672,7 +714,10 @@
       <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -689,7 +734,10 @@
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -706,7 +754,10 @@
       <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -723,7 +774,10 @@
       <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -740,7 +794,10 @@
       <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -757,7 +814,10 @@
       <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -774,8 +834,96 @@
       <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all upper div cs requirements
</commit_message>
<xml_diff>
--- a/CourseInformation.xlsx
+++ b/CourseInformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Latisha/Desktop/transferify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37856D1C-E57B-E949-A30A-FAE4EE04E56F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ECC96D-5EB0-F447-BB11-C22652BA23AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{799547F4-8573-6E46-8325-07C6A5C91E50}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>Class Name</t>
   </si>
@@ -190,16 +190,103 @@
   </si>
   <si>
     <t>Math 31A, Math 31B, Math 32A, Math 32B, Math 33A, Physics 1A, Physics 1B, Physics 1C</t>
+  </si>
+  <si>
+    <t>CS 111</t>
+  </si>
+  <si>
+    <t>CS 118</t>
+  </si>
+  <si>
+    <t>CS 131</t>
+  </si>
+  <si>
+    <t>CS M151B</t>
+  </si>
+  <si>
+    <t>CS M152A</t>
+  </si>
+  <si>
+    <t>CS 180</t>
+  </si>
+  <si>
+    <t>CS 181</t>
+  </si>
+  <si>
+    <t>CS 130</t>
+  </si>
+  <si>
+    <t>CS 152B</t>
+  </si>
+  <si>
+    <t>Upper Division CS Requirement</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, CS 33, CS 35L</t>
+  </si>
+  <si>
+    <t>Introduction to operating systems design and evaluation. Computer software systems performance, robustness, and functionality. Kernel structure, bootstrapping, input/output (I/O) devices and interrupts. Processes and threads; address spaces, memory management, and virtual memory. Scheduling, synchronization. File systems: layout, performance, robustness. Distributed systems: networking, remote procedure call (RPC), asynchronous RPC, distributed file systems, transactions. Protection and security. Exercises involving applications using, and internals of, real-world operating systems.</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, CS 33, CS 35L, CS 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Introduction to design and performance evaluation of computer networks, including such topics as what protocols are, layered network architecture, Internet protocol architecture, network applications, transport protocols, routing algorithms and protocols, internetworking, congestion control, and link layer protocols including Ethernet and wireless channels.</t>
+  </si>
+  <si>
+    <t>Basic concepts in design and use of programming languages, including abstraction, modularity, control mechanisms, types, declarations, syntax, and semantics. Study of several different language paradigms, including functional, object-oriented, and logic programming.</t>
+  </si>
+  <si>
+    <t>Stats Requirement</t>
+  </si>
+  <si>
+    <t>Computer system organization and design, implementation of CPU datapath and control, instruction set design, memory hierarchy (caches, main memory, virtual memory) organization and management, input/output subsystems (bus structures, interrupts, DMA), performance evaluation, pipelined processors.</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, CS 33, CS M51A</t>
+  </si>
+  <si>
+    <t>Hands-on design, implementation, and debugging of digital logic circuits, use of computer-aided design tools for schematic capture and simulation, implementation of complex circuits using programmed array logic, design projects.</t>
+  </si>
+  <si>
+    <t>*Fulfills Same Requirement as CS 130* Limited to seniors. Design and implementation of complex digital subsystems using field-programmable gate arrays (e.g., processors, special-purpose processors, device controllers, and input/output interfaces). Students work in teams to develop and implement designs and to document and give oral presentations of their work.</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, CS 33, CS M51A, CS 151B</t>
+  </si>
+  <si>
+    <t>*Fulfills Same Requirement as CS 152B* Structured programming, program specification, program proving, modularity, abstract data types, composite design, software tools, software control systems, program testing, team programming.</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, CS 33, CS 35L, CS 111, CS 131</t>
+  </si>
+  <si>
+    <t>Introduction to design and analysis of algorithms. Design techniques (divide-and-conquer, greedy method, dynamic programming), selection of prototypical algorithms, choice of data structures and representations, complexity measures (time, space, upper, lower bounds, asymptotic complexity), NP-completeness.</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, Math 31A, Math 31B, Math 61</t>
+  </si>
+  <si>
+    <t>Grammars, automata, and languages. Finite-state languages and finite-state automata. Context-free languages and pushdown story automata. Unrestricted rewriting systems, recursively enumerable and recursive languages, and Turing machines. Closure properties, pumping lemmas, and decision algorithms. Introduction to computability.</t>
+  </si>
+  <si>
+    <t>CS 31, CS 32, Math 31A, Math 31B, Math 62, CS 181</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -544,19 +631,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB62880F-4327-8B45-B967-BF103E8C0F94}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="29.5" style="1" customWidth="1"/>
   </cols>
@@ -581,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -601,7 +688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="122" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -621,7 +708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -641,7 +728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -661,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -681,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -781,7 +868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -821,7 +908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -841,7 +928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -854,11 +941,14 @@
       <c r="D15" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -870,6 +960,9 @@
       </c>
       <c r="D16" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>46</v>
@@ -888,6 +981,9 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>47</v>
       </c>
@@ -905,11 +1001,14 @@
       <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -922,11 +1021,200 @@
       <c r="D19" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="20" spans="1:6" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>